<commit_message>
Updates to the Discrete Summary Sample spreadsheets for Irminger and Pioneer arrays.
</commit_message>
<xml_diff>
--- a/Ship_data/Pioneer/Pioneer-04/Pioneer-04_Leg-1_AT-27A_Discrete_Summary_2019-06-05_ver_1-01_.xlsx
+++ b/Ship_data/Pioneer/Pioneer-04/Pioneer-04_Leg-1_AT-27A_Discrete_Summary_2019-06-05_ver_1-01_.xlsx
@@ -1522,10 +1522,10 @@
   </sheetPr>
   <dimension ref="A1:BW191"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="BI1" activeCellId="0" sqref="BI1"/>
-      <selection pane="bottomLeft" activeCell="BO191" activeCellId="0" sqref="BO191"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>